<commit_message>
changes 1. added nanoid and editable Exchange rate in invoice frontend 2. changes in excel invoice 3.added undo revoke txn feature
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D62C1A-DBAB-47AC-8362-F1E3262226D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF26F80D-8DDB-4B23-BF97-C1A8C2A0CC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Customer Name</t>
   </si>
@@ -230,9 +230,6 @@
   <si>
     <t>Purchase of renewable attributes for I-REC
 (20028.63 units at INR 51.68124 per unit)</t>
-  </si>
-  <si>
-    <t>Twelve Lakh Twenty one Thousand Four Hundred and Twenty Three Only</t>
   </si>
 </sst>
 </file>
@@ -694,6 +691,30 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -712,9 +733,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -723,27 +741,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1058,7 +1055,7 @@
   <dimension ref="A1:S66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1081,21 +1078,21 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1"/>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -1154,10 +1151,10 @@
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
       <c r="P4" s="10"/>
@@ -1177,10 +1174,10 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
       <c r="P5" s="10"/>
@@ -1221,11 +1218,11 @@
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
-      <c r="H7" s="74" t="s">
+      <c r="H7" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14"/>
@@ -1563,11 +1560,11 @@
     </row>
     <row r="22" spans="2:19" ht="34.200000000000003" customHeight="1">
       <c r="B22" s="7"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
@@ -1695,33 +1692,33 @@
     </row>
     <row r="28" spans="2:19" ht="21" customHeight="1">
       <c r="B28" s="7"/>
-      <c r="C28" s="64" t="s">
+      <c r="C28" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="70" t="s">
+      <c r="D28" s="60"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="70" t="s">
+      <c r="G28" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="64" t="s">
+      <c r="H28" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64" t="s">
+      <c r="I28" s="60"/>
+      <c r="J28" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64" t="s">
+      <c r="K28" s="60"/>
+      <c r="L28" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="71"/>
-      <c r="N28" s="71" t="s">
+      <c r="M28" s="62"/>
+      <c r="N28" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="O28" s="72"/>
+      <c r="O28" s="63"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
@@ -1729,11 +1726,11 @@
     </row>
     <row r="29" spans="2:19" ht="18">
       <c r="B29" s="7"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
       <c r="H29" s="22" t="s">
         <v>14</v>
       </c>
@@ -1785,11 +1782,11 @@
     </row>
     <row r="31" spans="2:19" ht="99.9" customHeight="1">
       <c r="B31" s="7"/>
-      <c r="C31" s="61" t="s">
+      <c r="C31" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="D31" s="62"/>
-      <c r="E31" s="63"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="71"/>
       <c r="F31" s="29" t="s">
         <v>48</v>
       </c>
@@ -1928,12 +1925,12 @@
     </row>
     <row r="37" spans="2:19" ht="18">
       <c r="B37" s="7"/>
-      <c r="C37" s="64" t="s">
+      <c r="C37" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="39">
         <f>SUM(G30:G36)</f>
         <v>1035104.4339012001</v>
@@ -2017,16 +2014,14 @@
       <c r="E40" s="9"/>
       <c r="F40" s="11"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="I40" s="60"/>
-      <c r="J40" s="60"/>
-      <c r="K40" s="60"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="60"/>
-      <c r="N40" s="60"/>
-      <c r="O40" s="60"/>
+      <c r="H40" s="68"/>
+      <c r="I40" s="68"/>
+      <c r="J40" s="68"/>
+      <c r="K40" s="68"/>
+      <c r="L40" s="68"/>
+      <c r="M40" s="68"/>
+      <c r="N40" s="68"/>
+      <c r="O40" s="68"/>
       <c r="P40" s="10"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
@@ -2061,14 +2056,14 @@
       <c r="E42" s="9"/>
       <c r="F42" s="11"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="65"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="65"/>
-      <c r="M42" s="67"/>
-      <c r="N42" s="65"/>
-      <c r="O42" s="66"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="74"/>
+      <c r="N42" s="72"/>
+      <c r="O42" s="73"/>
       <c r="P42" s="10"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
@@ -2306,59 +2301,59 @@
     </row>
     <row r="54" spans="2:19" ht="15" customHeight="1">
       <c r="B54" s="7"/>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
-      <c r="L54" s="58"/>
-      <c r="M54" s="58"/>
-      <c r="N54" s="58"/>
-      <c r="O54" s="58"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="66"/>
+      <c r="F54" s="66"/>
+      <c r="G54" s="66"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="66"/>
+      <c r="K54" s="66"/>
+      <c r="L54" s="66"/>
+      <c r="M54" s="66"/>
+      <c r="N54" s="66"/>
+      <c r="O54" s="66"/>
       <c r="P54" s="10"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
     </row>
     <row r="55" spans="2:19" ht="18">
       <c r="B55" s="7"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="58"/>
-      <c r="F55" s="58"/>
-      <c r="G55" s="58"/>
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
-      <c r="J55" s="58"/>
-      <c r="K55" s="58"/>
-      <c r="L55" s="58"/>
-      <c r="M55" s="58"/>
-      <c r="N55" s="58"/>
-      <c r="O55" s="58"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="66"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="66"/>
+      <c r="G55" s="66"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="66"/>
+      <c r="J55" s="66"/>
+      <c r="K55" s="66"/>
+      <c r="L55" s="66"/>
+      <c r="M55" s="66"/>
+      <c r="N55" s="66"/>
+      <c r="O55" s="66"/>
       <c r="P55" s="10"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
     <row r="56" spans="2:19" ht="18">
       <c r="B56" s="7"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="58"/>
-      <c r="G56" s="58"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
-      <c r="J56" s="58"/>
-      <c r="K56" s="58"/>
-      <c r="L56" s="58"/>
-      <c r="M56" s="58"/>
-      <c r="N56" s="58"/>
-      <c r="O56" s="58"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="66"/>
+      <c r="K56" s="66"/>
+      <c r="L56" s="66"/>
+      <c r="M56" s="66"/>
+      <c r="N56" s="66"/>
+      <c r="O56" s="66"/>
       <c r="P56" s="10"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
@@ -2366,19 +2361,19 @@
     </row>
     <row r="57" spans="2:19" ht="18">
       <c r="B57" s="7"/>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
-      <c r="E57" s="58"/>
-      <c r="F57" s="58"/>
-      <c r="G57" s="58"/>
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
-      <c r="J57" s="58"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="58"/>
-      <c r="N57" s="58"/>
-      <c r="O57" s="58"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="66"/>
+      <c r="G57" s="66"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="66"/>
+      <c r="L57" s="66"/>
+      <c r="M57" s="66"/>
+      <c r="N57" s="66"/>
+      <c r="O57" s="66"/>
       <c r="P57" s="10"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
@@ -2386,19 +2381,19 @@
     </row>
     <row r="58" spans="2:19" ht="23.25" customHeight="1">
       <c r="B58" s="7"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="58"/>
-      <c r="N58" s="58"/>
-      <c r="O58" s="58"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="66"/>
+      <c r="K58" s="66"/>
+      <c r="L58" s="66"/>
+      <c r="M58" s="66"/>
+      <c r="N58" s="66"/>
+      <c r="O58" s="66"/>
       <c r="P58" s="10"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
@@ -2406,19 +2401,19 @@
     </row>
     <row r="59" spans="2:19" ht="23.25" customHeight="1">
       <c r="B59" s="7"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="58"/>
-      <c r="F59" s="58"/>
-      <c r="G59" s="58"/>
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
-      <c r="J59" s="58"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="58"/>
-      <c r="N59" s="58"/>
-      <c r="O59" s="58"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66"/>
+      <c r="E59" s="66"/>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="66"/>
+      <c r="K59" s="66"/>
+      <c r="L59" s="66"/>
+      <c r="M59" s="66"/>
+      <c r="N59" s="66"/>
+      <c r="O59" s="66"/>
       <c r="P59" s="10"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
@@ -2426,19 +2421,19 @@
     </row>
     <row r="60" spans="2:19" ht="23.25" customHeight="1">
       <c r="B60" s="7"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="58"/>
-      <c r="F60" s="58"/>
-      <c r="G60" s="58"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
-      <c r="J60" s="58"/>
-      <c r="K60" s="58"/>
-      <c r="L60" s="58"/>
-      <c r="M60" s="58"/>
-      <c r="N60" s="58"/>
-      <c r="O60" s="58"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="66"/>
+      <c r="L60" s="66"/>
+      <c r="M60" s="66"/>
+      <c r="N60" s="66"/>
+      <c r="O60" s="66"/>
       <c r="P60" s="10"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
@@ -2446,19 +2441,19 @@
     </row>
     <row r="61" spans="2:19" ht="23.25" customHeight="1">
       <c r="B61" s="7"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
-      <c r="E61" s="58"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
-      <c r="J61" s="58"/>
-      <c r="K61" s="58"/>
-      <c r="L61" s="58"/>
-      <c r="M61" s="58"/>
-      <c r="N61" s="58"/>
-      <c r="O61" s="58"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="L61" s="66"/>
+      <c r="M61" s="66"/>
+      <c r="N61" s="66"/>
+      <c r="O61" s="66"/>
       <c r="P61" s="10"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
@@ -2506,21 +2501,21 @@
     </row>
     <row r="64" spans="2:19" ht="18" hidden="1">
       <c r="B64" s="7"/>
-      <c r="C64" s="59" t="s">
+      <c r="C64" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D64" s="59"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="59"/>
-      <c r="G64" s="59"/>
-      <c r="H64" s="59"/>
-      <c r="I64" s="59"/>
-      <c r="J64" s="59"/>
-      <c r="K64" s="59"/>
-      <c r="L64" s="59"/>
-      <c r="M64" s="59"/>
-      <c r="N64" s="59"/>
-      <c r="O64" s="59"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="67"/>
+      <c r="F64" s="67"/>
+      <c r="G64" s="67"/>
+      <c r="H64" s="67"/>
+      <c r="I64" s="67"/>
+      <c r="J64" s="67"/>
+      <c r="K64" s="67"/>
+      <c r="L64" s="67"/>
+      <c r="M64" s="67"/>
+      <c r="N64" s="67"/>
+      <c r="O64" s="67"/>
       <c r="P64" s="10"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
@@ -2528,21 +2523,21 @@
     </row>
     <row r="65" spans="2:19" ht="18" hidden="1">
       <c r="B65" s="7"/>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="68" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="60"/>
-      <c r="J65" s="60"/>
-      <c r="K65" s="60"/>
-      <c r="L65" s="60"/>
-      <c r="M65" s="60"/>
-      <c r="N65" s="60"/>
-      <c r="O65" s="60"/>
+      <c r="D65" s="68"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="68"/>
+      <c r="H65" s="68"/>
+      <c r="I65" s="68"/>
+      <c r="J65" s="68"/>
+      <c r="K65" s="68"/>
+      <c r="L65" s="68"/>
+      <c r="M65" s="68"/>
+      <c r="N65" s="68"/>
+      <c r="O65" s="68"/>
       <c r="P65" s="10"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
@@ -2570,6 +2565,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C54:O61"/>
+    <mergeCell ref="C64:O64"/>
+    <mergeCell ref="C65:O65"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="H40:O40"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
     <mergeCell ref="B1:P1"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="J5:M5"/>
@@ -2582,16 +2587,6 @@
     <mergeCell ref="N28:O28"/>
     <mergeCell ref="C22:G22"/>
     <mergeCell ref="H7:J7"/>
-    <mergeCell ref="C54:O61"/>
-    <mergeCell ref="C64:O64"/>
-    <mergeCell ref="C65:O65"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="H40:O40"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" orientation="portrait" r:id="rId1"/>

</xml_diff>